<commit_message>
Modif répartition des tâches
Étant donné que le travail est à finir pour jeudi (un jour avant la remise), j’ai modifié la répartition des tâches (en ce qui me concerne) : cela ne sert à rien qu’on soit à 2 sur un bogue.

Je viens de finir la BD (data/vino2.sql), du coup cela correspond au Story ID 318829 (improvement: revoir la structure des données pour avoir au moins 1 cellier par usager)

Je vais regarder la modification d’une bouteille dans le cellier.
</commit_message>
<xml_diff>
--- a/tableur/web_base-backlog_items_1548104231.xlsx
+++ b/tableur/web_base-backlog_items_1548104231.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10123"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/MAMP/htdocs/vinoGroupe/tableur/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E5673643-4063-C44D-8FB2-B0E108EECF36}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="38160" windowHeight="22440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="41">
   <si>
     <t>Story ID</t>
   </si>
@@ -146,7 +152,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="##0"/>
   </numFmts>
@@ -257,7 +263,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -290,9 +296,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -325,6 +348,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -500,21 +540,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" zoomScale="151" zoomScaleNormal="151" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="19.28515625" customWidth="1"/>
-    <col min="3" max="3" width="60.42578125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="94.140625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="19.33203125" customWidth="1"/>
+    <col min="3" max="3" width="60.5" style="4" customWidth="1"/>
+    <col min="4" max="4" width="94.1640625" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -528,7 +568,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>317929</v>
       </c>
@@ -544,11 +584,8 @@
       <c r="E2" t="s">
         <v>37</v>
       </c>
-      <c r="F2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>318830</v>
       </c>
@@ -568,7 +605,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>317927</v>
       </c>
@@ -581,8 +618,11 @@
       <c r="D4" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>317926</v>
       </c>
@@ -596,7 +636,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>318829</v>
       </c>
@@ -609,8 +649,11 @@
       <c r="D6" s="4" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>317930</v>
       </c>
@@ -624,7 +667,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>317931</v>
       </c>
@@ -638,7 +681,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>317933</v>
       </c>
@@ -652,7 +695,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>317934</v>
       </c>
@@ -666,7 +709,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>317935</v>
       </c>
@@ -680,7 +723,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>317936</v>
       </c>
@@ -694,7 +737,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>317937</v>
       </c>
@@ -708,7 +751,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>317938</v>
       </c>
@@ -722,7 +765,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>317939</v>
       </c>
@@ -736,7 +779,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="150" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="160" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>317940</v>
       </c>
@@ -750,7 +793,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>317941</v>
       </c>
@@ -764,7 +807,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>317942</v>
       </c>
@@ -778,7 +821,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>317943</v>
       </c>
@@ -792,7 +835,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>317945</v>
       </c>

</xml_diff>